<commit_message>
Adding array and string questions
</commit_message>
<xml_diff>
--- a/FAANG.xlsx
+++ b/FAANG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FAANG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{074917D3-4F77-47CA-8C7C-71FD02BEE2B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47180E6F-8EB0-4980-8C3C-1D95B590A357}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4AAF9615-271F-4AED-B9A4-DF7AEF9562AD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Array and Strings</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Find Majority Element</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/n3-repeated-number-array-o1-space/</t>
   </si>
 </sst>
 </file>
@@ -424,7 +427,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -464,7 +467,9 @@
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="5"/>
+      <c r="C4" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3">

</xml_diff>